<commit_message>
25.01.2021 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list 02-01-2021.xlsx
+++ b/2020/Others/Price list 02-01-2021.xlsx
@@ -282,7 +282,7 @@
     <t xml:space="preserve">   </t>
   </si>
   <si>
-    <t>Last Update(20-01-2021)</t>
+    <t>Last Update(25-01-2021)</t>
   </si>
 </sst>
 </file>
@@ -549,6 +549,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -594,9 +597,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 2" xfId="2"/>
@@ -636,7 +636,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -657,7 +657,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -863,7 +863,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1964,7 +1964,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2411,7 +2411,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2471,7 +2471,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2488,7 +2488,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2551,7 +2551,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2568,7 +2568,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2628,7 +2628,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2661,7 +2661,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2673,7 +2673,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2951,7 +2951,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2961,8 +2961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2980,56 +2980,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:15" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1">
       <c r="A5" s="12" t="s">
@@ -3744,7 +3744,7 @@
       <c r="H34" s="7">
         <v>8290</v>
       </c>
-      <c r="I34" s="32"/>
+      <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="8" t="s">
@@ -3941,33 +3941,33 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18" t="s">
+      <c r="B45" s="19"/>
+      <c r="C45" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="21" t="s">
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I45" s="22"/>
+      <c r="I45" s="23"/>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="19"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="24"/>
+      <c r="A46" s="20"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="25"/>
       <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10">

</xml_diff>